<commit_message>
Use approaches 2 and 4
</commit_message>
<xml_diff>
--- a/Kaggle links.xlsx
+++ b/Kaggle links.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sindhuja\Desktop\ML Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sindhuja\Documents\GitHub\Machine-Learning-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,6 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$8:$D$66</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -93,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +106,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,10 +154,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -150,8 +166,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,7 +485,7 @@
   <dimension ref="B1:BH66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +516,7 @@
       </c>
     </row>
     <row r="5" spans="2:60" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1"/>
@@ -561,12 +579,12 @@
       <c r="BH5" s="1"/>
     </row>
     <row r="6" spans="2:60" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:60" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -840,7 +858,10 @@
       <c r="D66" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>